<commit_message>
adjusted zeroshot modeling. running code again. 3000 sample
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C039064-88DA-4415-A715-C78323C89D85}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{405AE0FC-D2BB-454C-8674-B4AC236215E5}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>bad</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>zeroshot</t>
+  </si>
+  <si>
+    <t>15000s</t>
+  </si>
+  <si>
+    <t>auto!?</t>
   </si>
 </sst>
 </file>
@@ -455,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,95 +478,133 @@
     <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>3000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>200</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>50</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>3000</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>200</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>8</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6">
+        <v>200</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
good topics. now trying regular, nr topics null
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{405AE0FC-D2BB-454C-8674-B4AC236215E5}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA89064-8B75-407E-ABBA-E9490CF7395B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
+    <workbookView xWindow="588" yWindow="588" windowWidth="21660" windowHeight="11328" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>auto!?</t>
+  </si>
+  <si>
+    <t>zeroshot minsim</t>
+  </si>
+  <si>
+    <t>quite good</t>
+  </si>
+  <si>
+    <t>100+</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>3000s</t>
+  </si>
+  <si>
+    <t>seed words included</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>good</t>
   </si>
 </sst>
 </file>
@@ -467,23 +494,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -500,19 +529,25 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -531,20 +566,23 @@
       <c r="F4">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>13</v>
       </c>
-      <c r="I4">
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4">
         <v>50</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -563,20 +601,23 @@
       <c r="F5">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>13</v>
       </c>
-      <c r="I5">
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5">
         <v>8</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -595,17 +636,96 @@
       <c r="F6">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>0.7</v>
+      </c>
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="I6">
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6">
         <v>3</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>3000</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>0.3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>3000</v>
+      </c>
+      <c r="E8">
+        <v>200</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8">
+        <v>50</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying zeroshot with normal topic list now. 0.3 minsim. only change: seed words included
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA89064-8B75-407E-ABBA-E9490CF7395B}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{043AED9C-0629-4C2C-90EC-8D6203620D95}"/>
   <bookViews>
-    <workbookView xWindow="588" yWindow="588" windowWidth="21660" windowHeight="11328" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
+    <workbookView xWindow="936" yWindow="912" windowWidth="21660" windowHeight="11328" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -494,25 +494,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -547,7 +547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -582,7 +582,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -617,7 +617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -655,7 +655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -693,7 +693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -726,6 +726,38 @@
       </c>
       <c r="L8" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>3000</v>
+      </c>
+      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying huang topic list
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{043AED9C-0629-4C2C-90EC-8D6203620D95}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CD01552-0FF2-4490-8D16-23BE1DE7C1CD}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="912" windowWidth="21660" windowHeight="11328" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>good</t>
+  </si>
+  <si>
+    <t>zeroshot huang</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,6 +763,64 @@
         <v>115</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>3000</v>
+      </c>
+      <c r="E10">
+        <v>200</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>4700</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>3000</v>
+      </c>
+      <c r="E11">
+        <v>200</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated fitting script (pca for regular). updating zeroshot topic list. combining own and huang.
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CD01552-0FF2-4490-8D16-23BE1DE7C1CD}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6043DC56-52C1-41CF-A456-C1415431774A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>zeroshot huang</t>
+  </si>
+  <si>
+    <t>medium ( seems like topics get split up)</t>
+  </si>
+  <si>
+    <t>zeroshot huang combined with own</t>
   </si>
 </sst>
 </file>
@@ -497,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,6 +768,9 @@
       <c r="K9">
         <v>115</v>
       </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -794,6 +803,9 @@
       <c r="K10">
         <v>110</v>
       </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -814,11 +826,25 @@
       <c r="F11">
         <v>5</v>
       </c>
+      <c r="H11">
+        <v>2500</v>
+      </c>
       <c r="I11" t="s">
         <v>23</v>
       </c>
       <c r="J11" t="s">
         <v>27</v>
+      </c>
+      <c r="K11">
+        <v>115</v>
+      </c>
+      <c r="L11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying nr topics auto with huang +own zeroshot model.
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCC9A101-3724-4A4A-B20C-CA2909A9226A}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16ADE534-E089-4278-AB35-3E57D39269FF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -503,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,6 +868,26 @@
         <v>112</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>3000</v>
+      </c>
+      <c r="E13">
+        <v>200</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
also doing zeroshot huang own again. after analyzing this later, i might need to drop few topics.
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6674A28F-4505-4BD7-B9A9-0E6AEEA8165E}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F3EEB2B-D1FE-47A6-8DC7-7951AD21DB73}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -153,12 +153,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -173,8 +179,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +519,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,37 +716,38 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>3000</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>200</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>50</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -779,37 +787,38 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>3000</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>200</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>5</v>
       </c>
-      <c r="H10">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
         <v>4700</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="1">
         <v>110</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trying again with lower min cluster size
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F3EEB2B-D1FE-47A6-8DC7-7951AD21DB73}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA05A14C-5473-4A06-941F-B2DCF423065A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>.-&gt; zeroshot und auto nicht kombinieren!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3000s ca </t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,6 +921,41 @@
         <v>33</v>
       </c>
     </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>3000</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14">
+        <v>115</v>
+      </c>
+      <c r="L14" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
08 minsim was good trying 095 now
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA05A14C-5473-4A06-941F-B2DCF423065A}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C77F54A-3DFE-4EDF-BB65-28CDF42104E0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">3000s ca </t>
+  </si>
+  <si>
+    <t>pretty good</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,6 +959,40 @@
         <v>15</v>
       </c>
     </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <v>3000</v>
+      </c>
+      <c r="E15" s="1">
+        <v>200</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H15" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="1">
+        <v>112</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
trying zeroshot 095 minsim
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C77F54A-3DFE-4EDF-BB65-28CDF42104E0}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{438C188B-2ABD-4444-99AE-23C0E2E5FD2D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>pretty good</t>
+  </si>
+  <si>
+    <t>150+</t>
   </si>
 </sst>
 </file>
@@ -522,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,12 +989,44 @@
       <c r="J15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="1">
-        <v>112</v>
+      <c r="K15" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>35</v>
       </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1">
+        <v>3000</v>
+      </c>
+      <c r="E16" s="1">
+        <v>200</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="1">
+        <v>112</v>
+      </c>
+      <c r="L16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
similiarity threshold now in config. trying zeroshot with 01 minsim, and 03 sim threshold for merging. 4000 sample size. also updated final df creation. hopefully, needs check.
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{438C188B-2ABD-4444-99AE-23C0E2E5FD2D}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA98AD9F-19EB-4E2A-9C8D-1D4AE96FC81A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>150+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">worse than 08. topics getting too small </t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,9 +197,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,36 +1007,38 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1">
-        <v>3000</v>
-      </c>
-      <c r="E16" s="1">
-        <v>200</v>
-      </c>
-      <c r="F16" s="1">
-        <v>5</v>
-      </c>
-      <c r="G16" s="1">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E16" s="2">
+        <v>200</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2">
         <v>0.95</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <v>4000</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="2">
         <v>112</v>
       </c>
-      <c r="L16" s="1"/>
+      <c r="L16" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
topic labels not fixed yet. epsfxq_next cant create yet. now trying to change similarity computations, so that only calls from the past are taken into account.
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE469BD3-E210-4B40-BFF6-929541A19EF4}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F38DDF5-FF42-49B8-B835-6D140B5708A5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="41">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>medium, too many micro clusters, -1 is too large</t>
+  </si>
+  <si>
+    <t>.-&gt; das evtl nochmal mit auto trainieren</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1049,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1079,6 +1082,9 @@
       </c>
       <c r="L17" t="s">
         <v>39</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.0 minsim didnt work. trying the same with nr topics auto
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F38DDF5-FF42-49B8-B835-6D140B5708A5}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FC5C5B0-A237-4D11-BA43-54BF4AD54D4E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="42">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>.-&gt; das evtl nochmal mit auto trainieren</t>
+  </si>
+  <si>
+    <t>zeroshot huang combined with own (w/o marketing)</t>
   </si>
 </sst>
 </file>
@@ -544,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,6 +1090,126 @@
         <v>40</v>
       </c>
     </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E19" s="2">
+        <v>200</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>4000</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E20" s="2">
+        <v>200</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H20" s="2">
+        <v>4000</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E21" s="2">
+        <v>200</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="2">
+        <v>4000</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
+        <v>4000</v>
+      </c>
+      <c r="E22" s="2">
+        <v>200</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H22" s="2">
+        <v>4000</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
0.0 didnt work again. trying 0.05
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81A0ECAD-8C13-45DA-8BF1-1BF4793BF961}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64A9CD54-B8C8-4E4E-952E-AA3F82C3D439}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8928" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="43">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -231,6 +231,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L20" sqref="A20:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,36 +1130,38 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
         <v>4000</v>
       </c>
-      <c r="E20" s="2">
-        <v>200</v>
-      </c>
-      <c r="F20" s="2">
-        <v>5</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="E20" s="1">
+        <v>200</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1">
         <v>0.25</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>4000</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K20" s="2">
+      <c r="J20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="1">
         <v>89</v>
       </c>
-      <c r="L20" s="2"/>
+      <c r="L20" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
@@ -1187,7 +1193,9 @@
       <c r="K21" s="2">
         <v>198</v>
       </c>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -1219,7 +1227,9 @@
       <c r="K22" s="2">
         <v>193</v>
       </c>
-      <c r="L22" s="2"/>
+      <c r="L22" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
trying run using cuml
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64A9CD54-B8C8-4E4E-952E-AA3F82C3D439}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{541B683E-C457-4FAD-896C-FBB7D2446865}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="44">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">representations very good; but only few outliers, outliers might be assigned to other topics. This needs check in the full workflow. </t>
   </si>
 </sst>
 </file>
@@ -231,10 +234,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -554,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="L20" sqref="A20:L20"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1231,6 +1230,75 @@
         <v>14</v>
       </c>
     </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <v>200</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>14000</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E24" s="1">
+        <v>200</v>
+      </c>
+      <c r="F24" s="1">
+        <v>5</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H24" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="1">
+        <v>14</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1st training worked fast with cuml (5000 sample, nr topics null). needs check. now training with 10k sample and nr topics auto and null
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{541B683E-C457-4FAD-896C-FBB7D2446865}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B504CE6-168A-4732-8C24-DDFEA1E821BA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="46">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t xml:space="preserve">representations very good; but only few outliers, outliers might be assigned to other topics. This needs check in the full workflow. </t>
+  </si>
+  <si>
+    <t>ab hier mit cuml</t>
+  </si>
+  <si>
+    <t>2900s</t>
   </si>
 </sst>
 </file>
@@ -553,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,6 +1305,43 @@
         <v>43</v>
       </c>
     </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>200</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
now trying zeroshot and regular 2500 on bertopic_training.py
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5294C0E6-8CB8-48F4-AD0B-9A4E34CC1D22}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12A73F2A-D1D3-4CAB-B74A-747E3742D5A2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>quite good, needs some merging prob. Results not as expected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ohne cuml </t>
+  </si>
+  <si>
+    <t>3300s</t>
+  </si>
+  <si>
+    <t>zeroshot minsim variert stark mit topic size!!!</t>
   </si>
 </sst>
 </file>
@@ -562,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="76" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,6 +1357,83 @@
         <v>46</v>
       </c>
     </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30">
+        <v>1000</v>
+      </c>
+      <c r="E30">
+        <v>200</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30">
+        <v>130</v>
+      </c>
+      <c r="L30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E31" s="2">
+        <v>200</v>
+      </c>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K31" s="2">
+        <v>145</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fitting script with reg 2500 40 topics
</commit_message>
<xml_diff>
--- a/model_training_tracking.xlsx
+++ b/model_training_tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9E1B6EB-A211-44EB-AE66-BBFB6595B089}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="8_{8F99C80A-D093-4BB5-9E5A-700AEF4472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6227F62-C346-4A3F-A113-07D289A2972D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1891C698-8948-476A-94E5-98137577C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="56">
   <si>
     <t>Model training tracking</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>nicht nr topics auto</t>
+  </si>
+  <si>
+    <t>5500s</t>
+  </si>
+  <si>
+    <t>4900s</t>
+  </si>
+  <si>
+    <t>5900s</t>
+  </si>
+  <si>
+    <t>medium (z.b. costs +earnings sind grouped)</t>
   </si>
 </sst>
 </file>
@@ -577,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052DAB51-BA3A-4629-8C33-B32CD9292071}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="76" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,6 +1489,172 @@
         <v>51</v>
       </c>
     </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E37" s="2">
+        <v>200</v>
+      </c>
+      <c r="F37" s="2">
+        <v>5</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K37" s="2">
+        <v>77</v>
+      </c>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E38" s="2">
+        <v>200</v>
+      </c>
+      <c r="F38" s="2">
+        <v>5</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K38" s="2">
+        <v>144</v>
+      </c>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E40">
+        <v>200</v>
+      </c>
+      <c r="F40">
+        <v>5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>53</v>
+      </c>
+      <c r="I40">
+        <v>20</v>
+      </c>
+      <c r="J40" t="s">
+        <v>27</v>
+      </c>
+      <c r="K40">
+        <v>20</v>
+      </c>
+      <c r="L40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E41">
+        <v>200</v>
+      </c>
+      <c r="F41">
+        <v>5</v>
+      </c>
+      <c r="H41" t="s">
+        <v>53</v>
+      </c>
+      <c r="I41">
+        <v>30</v>
+      </c>
+      <c r="J41" t="s">
+        <v>27</v>
+      </c>
+      <c r="K41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E42">
+        <v>200</v>
+      </c>
+      <c r="F42">
+        <v>5</v>
+      </c>
+      <c r="H42" t="s">
+        <v>53</v>
+      </c>
+      <c r="I42">
+        <v>40</v>
+      </c>
+      <c r="J42" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42">
+        <v>40</v>
+      </c>
+      <c r="L42" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>